<commit_message>
Actualización de archivos JSON y scripts 24 de noviembre
</commit_message>
<xml_diff>
--- a/Alfa.xlsx
+++ b/Alfa.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9555"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="EN PROCESO (Alfa)" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="376">
   <si>
     <t>Asignado a</t>
   </si>
@@ -1262,7 +1262,13 @@
 Se crea funcionalidad de cierre masivo.
 El módulo se divide en dos pestañas: gestión de casos y el histórico.
 13/11/2025: Se continua con la creacion de la pestaña de historico, donde se debe visualizar los casos cerrados y permitir exportar los formatos que se reportan a cada una de las areas correspondientes como PLUS, SIPREN y Tesoreria.
-Se sostiene reunión con el área de previsionales para mostar los avances, pendiente por parte del cliente validar la información de los formatos si están acordes con el proceso.</t>
+Se sostiene reunión con el área de previsionales para mostar los avances, pendiente por parte del cliente validar la información de los formatos si están acordes con el proceso.
+14/11/2025: Se termina opciòn de històrico de honorarios jurìdicos, con cada una de las funcionalidades requeridas como descargar los formatos de SIPREN, Plus y Tesorerìa, se agrego funcionalidad de notificar cuando se hace el cierre manual.
+18/11/2025: Reuniòn con el cliente para probar el mòdulo, realizando el cargue de la prefactura, cierre y gestiòn del proceso. De esta reunion surgieron recomendaciones y ajustes:
+1. Que al descargar la prefactura baje tal cual como sube y permita agregar el estado "OBJETAR" y "PAGAR", que se agregue la causal de devoluciòn.
+2. Que cuando se cargue nuevamente cambie el estado y la causal masivamente.
+19/11/2025: Se continua realizando los ajustes solicitados en la reuniòn.
+Se realiza sesiòn y se presenta nuevamente el mòdulo y genero issu en el cargue. Donde sale consumo de memoria. Se revisa el problema el cual se sigio presnetando hasta el 20 de noviembre, por lo que se requiriò una refactorizaciòn en el cargue..</t>
   </si>
   <si>
     <t>REN_2025_06</t>
@@ -1372,6 +1378,64 @@
   </si>
   <si>
     <t>13/11/2025: Solicitan habilitar gestión de documentos para que muestre todos los documentos de todos los beneficiarios y no solo prioridad de unas rentas en particular, para unos temas de auditoría. Ya finalizada la auditoría se realizó actualización y reversión del ajuste.</t>
+  </si>
+  <si>
+    <t>Img_2025_025</t>
+  </si>
+  <si>
+    <t>Se requiere soporte para despliegue a producciòn y pruebas del modulo certificados masivos</t>
+  </si>
+  <si>
+    <t>18/11/2025: Se brinda soporte a Wilson Aponte para bajar cambios de este modulo nuevo en producciòn y en pruebas. Durante el proceso se presento inconveniente con el repositorio debido a connection time out.</t>
+  </si>
+  <si>
+    <t>SST_2025_015</t>
+  </si>
+  <si>
+    <t>Validar incidencia reportada por el àrea en cierre de ordenes de servicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19/11/2025: El àrea reporta lentitud en el proceso de auditoria de prefactura, donde se generaba un error 500. Este error indicaba que el servidor se quedo sin espacio, lo que impedia finalizar o cerrar OS, se procede a dar soluciòn reubicando los soportes y actas a un disco con mas capacidad.
+</t>
+  </si>
+  <si>
+    <t>SST_2025_016</t>
+  </si>
+  <si>
+    <t>Validar incidencia reportada por el àrea para el cargue de documentos por parte de los proveedores</t>
+  </si>
+  <si>
+    <t>20/11/2025: Nos reportan incidencia en el cargue de los soportes por parte de los proveedores, por lo cual se procediò a corregir el tema debido a la contingencia reportada el dia anterior, no se tuvo en cuenta los permisos de carpeta, se corrige y se notifica al cliente.</t>
+  </si>
+  <si>
+    <t>PRV_2025_034</t>
+  </si>
+  <si>
+    <t>Informe Anexo 1</t>
+  </si>
+  <si>
+    <t>Se requiere reajustar la vista del requerimiento</t>
+  </si>
+  <si>
+    <t>20/11/2025: Se refactoriza script de anexo 1, acorde a lo enviado por el àrea para ser ajustadocon base a la lògica solicitada. Se realiza el ajuste pertinente , sin embargo se presenta inconsistencia con la informaciòn, en espera de respuesta del àrea para finalizar el tema.</t>
+  </si>
+  <si>
+    <t>Img_2025_026</t>
+  </si>
+  <si>
+    <t>Soporte modulo Imaginex</t>
+  </si>
+  <si>
+    <t>Se requiere validaciòn en cambio de contraseña, arroja error</t>
+  </si>
+  <si>
+    <t>21/11/2025: Se brindo apoyo para el cambio de contraseña a la Doc Claudia Vargas, ya que generaba error al redirigirla en la opciòn de cambiar la contraseña</t>
+  </si>
+  <si>
+    <t>Img_2025_027</t>
+  </si>
+  <si>
+    <t>20/11/2025: Se monta caso a tecnologia notificando que nos encontramos sin conexiòn con el repositorio. En horas de la tarde en sesiòn con Jenry Henao, nos manifesto que este inconveniente se presento debido a una falla en github, lo que impedia realizar Pull. Una vez restabecido el servicio, se procediò a desplegar los cambios en pruebas y producciòn.</t>
   </si>
 </sst>
 </file>
@@ -2277,7 +2341,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla" displayName="Tabla" ref="A1:R1018">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla" displayName="Tabla" ref="A1:R1024">
   <tableColumns count="18">
     <tableColumn id="1" name="Asignado a"/>
     <tableColumn id="2" name="# REQ"/>
@@ -2568,10 +2632,10 @@
   <sheetPr>
     <tabColor rgb="FFCC0000"/>
   </sheetPr>
-  <dimension ref="A1:R1019"/>
+  <dimension ref="A1:R1025"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -4669,7 +4733,7 @@
       <c r="L43" s="68"/>
       <c r="M43" s="69">
         <f ca="1">IF(ISBLANK(L43), NETWORKDAYS(J43, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J43, L43, [1]Hoja2!$A$1:$A$18))</f>
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="N43" s="70"/>
       <c r="O43" s="71"/>
@@ -6893,7 +6957,7 @@
       <c r="L89" s="68"/>
       <c r="M89" s="69">
         <f ca="1">IF(ISBLANK(L89), NETWORKDAYS(J89, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J89, L89, [1]Hoja2!$A$1:$A$18))</f>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="N89" s="70"/>
       <c r="O89" s="71"/>
@@ -7418,7 +7482,7 @@
       <c r="L100" s="75"/>
       <c r="M100" s="90">
         <f ca="1">IF(ISBLANK(L100), NETWORKDAYS(J100, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J100, L100, [1]Hoja2!$A$1:$A$18))</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N100" s="91"/>
       <c r="O100" s="92"/>
@@ -7480,124 +7544,296 @@
       <c r="R101" s="72"/>
     </row>
     <row r="102" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A102" s="107"/>
-      <c r="B102" s="108"/>
-      <c r="C102" s="109"/>
-      <c r="D102" s="110"/>
-      <c r="E102" s="111"/>
-      <c r="F102" s="110"/>
-      <c r="G102" s="112"/>
-      <c r="H102" s="112"/>
-      <c r="I102" s="113"/>
-      <c r="J102" s="114"/>
-      <c r="K102" s="114"/>
-      <c r="L102" s="114"/>
-      <c r="M102" s="115"/>
-      <c r="N102" s="113"/>
-      <c r="O102" s="116"/>
-      <c r="P102" s="117"/>
-      <c r="Q102" s="118"/>
-      <c r="R102" s="119"/>
+      <c r="A102" s="95" t="s">
+        <v>18</v>
+      </c>
+      <c r="B102" s="81" t="s">
+        <v>357</v>
+      </c>
+      <c r="C102" s="96" t="s">
+        <v>331</v>
+      </c>
+      <c r="D102" s="63" t="s">
+        <v>358</v>
+      </c>
+      <c r="E102" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="F102" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="G102" s="82">
+        <v>100</v>
+      </c>
+      <c r="H102" s="78"/>
+      <c r="I102" s="102">
+        <v>45979</v>
+      </c>
+      <c r="J102" s="103">
+        <v>45979</v>
+      </c>
+      <c r="K102" s="103">
+        <v>45979</v>
+      </c>
+      <c r="L102" s="103">
+        <v>45979</v>
+      </c>
+      <c r="M102" s="98">
+        <f ca="1">IF(ISBLANK(L102), NETWORKDAYS(J102, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J102, L102, [1]Hoja2!$A$1:$A$18))</f>
+        <v>1</v>
+      </c>
+      <c r="N102" s="70"/>
+      <c r="O102" s="71"/>
+      <c r="P102" s="104" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q102" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="R102" s="80"/>
     </row>
     <row r="103" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A103" s="107"/>
-      <c r="B103" s="108"/>
-      <c r="C103" s="109"/>
-      <c r="D103" s="110"/>
-      <c r="E103" s="111"/>
-      <c r="F103" s="110"/>
-      <c r="G103" s="112"/>
-      <c r="H103" s="112"/>
-      <c r="I103" s="113"/>
-      <c r="J103" s="114"/>
-      <c r="K103" s="114"/>
-      <c r="L103" s="114"/>
-      <c r="M103" s="120"/>
-      <c r="N103" s="113"/>
-      <c r="O103" s="116"/>
-      <c r="P103" s="119"/>
-      <c r="Q103" s="118"/>
-      <c r="R103" s="119"/>
+      <c r="A103" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="B103" s="64" t="s">
+        <v>360</v>
+      </c>
+      <c r="C103" s="86" t="s">
+        <v>328</v>
+      </c>
+      <c r="D103" s="100" t="s">
+        <v>361</v>
+      </c>
+      <c r="E103" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="F103" s="99" t="s">
+        <v>22</v>
+      </c>
+      <c r="G103" s="88">
+        <v>100</v>
+      </c>
+      <c r="H103" s="89"/>
+      <c r="I103" s="94">
+        <v>45980</v>
+      </c>
+      <c r="J103" s="75">
+        <v>45980</v>
+      </c>
+      <c r="K103" s="75">
+        <v>45980</v>
+      </c>
+      <c r="L103" s="75">
+        <v>45980</v>
+      </c>
+      <c r="M103" s="90">
+        <f ca="1">IF(ISBLANK(L103), NETWORKDAYS(J103, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J103, L103, [1]Hoja2!$A$1:$A$18))</f>
+        <v>1</v>
+      </c>
+      <c r="N103" s="91"/>
+      <c r="O103" s="92"/>
+      <c r="P103" s="76" t="s">
+        <v>362</v>
+      </c>
+      <c r="Q103" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="R103" s="72"/>
     </row>
     <row r="104" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A104" s="107"/>
-      <c r="B104" s="108"/>
-      <c r="C104" s="109"/>
-      <c r="D104" s="110"/>
-      <c r="E104" s="111"/>
-      <c r="F104" s="110"/>
-      <c r="G104" s="112"/>
-      <c r="H104" s="112"/>
-      <c r="I104" s="113"/>
-      <c r="J104" s="114"/>
-      <c r="K104" s="114"/>
-      <c r="L104" s="114"/>
-      <c r="M104" s="120"/>
-      <c r="N104" s="113"/>
-      <c r="O104" s="116"/>
-      <c r="P104" s="119"/>
-      <c r="Q104" s="118"/>
-      <c r="R104" s="119"/>
+      <c r="A104" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="B104" s="64" t="s">
+        <v>363</v>
+      </c>
+      <c r="C104" s="86" t="s">
+        <v>328</v>
+      </c>
+      <c r="D104" s="100" t="s">
+        <v>364</v>
+      </c>
+      <c r="E104" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="F104" s="99" t="s">
+        <v>22</v>
+      </c>
+      <c r="G104" s="88">
+        <v>100</v>
+      </c>
+      <c r="H104" s="89"/>
+      <c r="I104" s="94">
+        <v>45981</v>
+      </c>
+      <c r="J104" s="75">
+        <v>45981</v>
+      </c>
+      <c r="K104" s="75">
+        <v>45981</v>
+      </c>
+      <c r="L104" s="75">
+        <v>45981</v>
+      </c>
+      <c r="M104" s="90">
+        <f ca="1">IF(ISBLANK(L104), NETWORKDAYS(J104, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J104, L104, [1]Hoja2!$A$1:$A$18))</f>
+        <v>1</v>
+      </c>
+      <c r="N104" s="91"/>
+      <c r="O104" s="92"/>
+      <c r="P104" s="76" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q104" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="R104" s="72"/>
     </row>
     <row r="105" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A105" s="107"/>
-      <c r="B105" s="108"/>
-      <c r="C105" s="109"/>
-      <c r="D105" s="110"/>
-      <c r="E105" s="111"/>
-      <c r="F105" s="110"/>
-      <c r="G105" s="112"/>
-      <c r="H105" s="112"/>
-      <c r="I105" s="113"/>
-      <c r="J105" s="114"/>
-      <c r="K105" s="114"/>
-      <c r="L105" s="114"/>
-      <c r="M105" s="120"/>
-      <c r="N105" s="113"/>
-      <c r="O105" s="116"/>
-      <c r="P105" s="119"/>
-      <c r="Q105" s="118"/>
-      <c r="R105" s="119"/>
+      <c r="A105" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="B105" s="64" t="s">
+        <v>366</v>
+      </c>
+      <c r="C105" s="86" t="s">
+        <v>367</v>
+      </c>
+      <c r="D105" s="93" t="s">
+        <v>368</v>
+      </c>
+      <c r="E105" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="F105" s="87" t="s">
+        <v>161</v>
+      </c>
+      <c r="G105" s="88">
+        <v>80</v>
+      </c>
+      <c r="H105" s="89"/>
+      <c r="I105" s="94">
+        <v>45981</v>
+      </c>
+      <c r="J105" s="75">
+        <v>45981</v>
+      </c>
+      <c r="K105" s="75">
+        <v>45989</v>
+      </c>
+      <c r="L105" s="75"/>
+      <c r="M105" s="90">
+        <f ca="1">IF(ISBLANK(L105), NETWORKDAYS(J105, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J105, L105, [1]Hoja2!$A$1:$A$18))</f>
+        <v>3</v>
+      </c>
+      <c r="N105" s="91"/>
+      <c r="O105" s="92"/>
+      <c r="P105" s="76" t="s">
+        <v>369</v>
+      </c>
+      <c r="Q105" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="R105" s="72"/>
     </row>
     <row r="106" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A106" s="107"/>
-      <c r="B106" s="108"/>
-      <c r="C106" s="109"/>
-      <c r="D106" s="110"/>
-      <c r="E106" s="111"/>
-      <c r="F106" s="110"/>
-      <c r="G106" s="112"/>
-      <c r="H106" s="112"/>
-      <c r="I106" s="113"/>
-      <c r="J106" s="114"/>
-      <c r="K106" s="114"/>
-      <c r="L106" s="114"/>
-      <c r="M106" s="120"/>
-      <c r="N106" s="113"/>
-      <c r="O106" s="116"/>
-      <c r="P106" s="119"/>
-      <c r="Q106" s="118"/>
-      <c r="R106" s="119"/>
+      <c r="A106" s="95" t="s">
+        <v>18</v>
+      </c>
+      <c r="B106" s="81" t="s">
+        <v>370</v>
+      </c>
+      <c r="C106" s="96" t="s">
+        <v>371</v>
+      </c>
+      <c r="D106" s="63" t="s">
+        <v>372</v>
+      </c>
+      <c r="E106" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="F106" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="G106" s="82">
+        <v>100</v>
+      </c>
+      <c r="H106" s="78"/>
+      <c r="I106" s="102">
+        <v>45982</v>
+      </c>
+      <c r="J106" s="103">
+        <v>45982</v>
+      </c>
+      <c r="K106" s="103">
+        <v>45982</v>
+      </c>
+      <c r="L106" s="103">
+        <v>45982</v>
+      </c>
+      <c r="M106" s="98">
+        <f ca="1">IF(ISBLANK(L106), NETWORKDAYS(J106, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J106, L106, [1]Hoja2!$A$1:$A$18))</f>
+        <v>1</v>
+      </c>
+      <c r="N106" s="70"/>
+      <c r="O106" s="71"/>
+      <c r="P106" s="104" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q106" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="R106" s="80"/>
     </row>
     <row r="107" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A107" s="107"/>
-      <c r="B107" s="108"/>
-      <c r="C107" s="109"/>
-      <c r="D107" s="110"/>
-      <c r="E107" s="111"/>
-      <c r="F107" s="110"/>
-      <c r="G107" s="112"/>
-      <c r="H107" s="112"/>
-      <c r="I107" s="113"/>
-      <c r="J107" s="114"/>
-      <c r="K107" s="114"/>
-      <c r="L107" s="114"/>
-      <c r="M107" s="120"/>
-      <c r="N107" s="113"/>
-      <c r="O107" s="116"/>
-      <c r="P107" s="119"/>
-      <c r="Q107" s="118"/>
-      <c r="R107" s="119"/>
+      <c r="A107" s="95" t="s">
+        <v>18</v>
+      </c>
+      <c r="B107" s="81" t="s">
+        <v>374</v>
+      </c>
+      <c r="C107" s="96" t="s">
+        <v>331</v>
+      </c>
+      <c r="D107" s="63" t="s">
+        <v>358</v>
+      </c>
+      <c r="E107" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="F107" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="G107" s="82">
+        <v>100</v>
+      </c>
+      <c r="H107" s="78"/>
+      <c r="I107" s="102">
+        <v>45981</v>
+      </c>
+      <c r="J107" s="103">
+        <v>45981</v>
+      </c>
+      <c r="K107" s="103">
+        <v>45981</v>
+      </c>
+      <c r="L107" s="103">
+        <v>45981</v>
+      </c>
+      <c r="M107" s="98">
+        <f ca="1">IF(ISBLANK(L107), NETWORKDAYS(J107, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J107, L107, [1]Hoja2!$A$1:$A$18))</f>
+        <v>1</v>
+      </c>
+      <c r="N107" s="70"/>
+      <c r="O107" s="71"/>
+      <c r="P107" s="104" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q107" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="R107" s="80"/>
     </row>
     <row r="108" spans="1:18" ht="29.25" customHeight="1">
       <c r="A108" s="107"/>
@@ -7612,10 +7848,10 @@
       <c r="J108" s="114"/>
       <c r="K108" s="114"/>
       <c r="L108" s="114"/>
-      <c r="M108" s="120"/>
+      <c r="M108" s="115"/>
       <c r="N108" s="113"/>
       <c r="O108" s="116"/>
-      <c r="P108" s="119"/>
+      <c r="P108" s="117"/>
       <c r="Q108" s="118"/>
       <c r="R108" s="119"/>
     </row>
@@ -7744,7 +7980,7 @@
       <c r="B115" s="108"/>
       <c r="C115" s="109"/>
       <c r="D115" s="110"/>
-      <c r="E115" s="121"/>
+      <c r="E115" s="111"/>
       <c r="F115" s="110"/>
       <c r="G115" s="112"/>
       <c r="H115" s="112"/>
@@ -7756,7 +7992,7 @@
       <c r="N115" s="113"/>
       <c r="O115" s="116"/>
       <c r="P115" s="119"/>
-      <c r="Q115" s="122"/>
+      <c r="Q115" s="118"/>
       <c r="R115" s="119"/>
     </row>
     <row r="116" spans="1:18" ht="29.25" customHeight="1">
@@ -7784,7 +8020,7 @@
       <c r="B117" s="108"/>
       <c r="C117" s="109"/>
       <c r="D117" s="110"/>
-      <c r="E117" s="121"/>
+      <c r="E117" s="111"/>
       <c r="F117" s="110"/>
       <c r="G117" s="112"/>
       <c r="H117" s="112"/>
@@ -7796,7 +8032,7 @@
       <c r="N117" s="113"/>
       <c r="O117" s="116"/>
       <c r="P117" s="119"/>
-      <c r="Q117" s="122"/>
+      <c r="Q117" s="118"/>
       <c r="R117" s="119"/>
     </row>
     <row r="118" spans="1:18" ht="29.25" customHeight="1">
@@ -7824,7 +8060,7 @@
       <c r="B119" s="108"/>
       <c r="C119" s="109"/>
       <c r="D119" s="110"/>
-      <c r="E119" s="121"/>
+      <c r="E119" s="111"/>
       <c r="F119" s="110"/>
       <c r="G119" s="112"/>
       <c r="H119" s="112"/>
@@ -7836,7 +8072,7 @@
       <c r="N119" s="113"/>
       <c r="O119" s="116"/>
       <c r="P119" s="119"/>
-      <c r="Q119" s="122"/>
+      <c r="Q119" s="118"/>
       <c r="R119" s="119"/>
     </row>
     <row r="120" spans="1:18" ht="29.25" customHeight="1">
@@ -25764,7 +26000,7 @@
       <c r="B1016" s="108"/>
       <c r="C1016" s="109"/>
       <c r="D1016" s="110"/>
-      <c r="E1016" s="123"/>
+      <c r="E1016" s="111"/>
       <c r="F1016" s="110"/>
       <c r="G1016" s="112"/>
       <c r="H1016" s="112"/>
@@ -25776,7 +26012,7 @@
       <c r="N1016" s="113"/>
       <c r="O1016" s="116"/>
       <c r="P1016" s="119"/>
-      <c r="Q1016" s="124"/>
+      <c r="Q1016" s="118"/>
       <c r="R1016" s="119"/>
     </row>
     <row r="1017" spans="1:18" ht="29.25" customHeight="1">
@@ -25784,7 +26020,7 @@
       <c r="B1017" s="108"/>
       <c r="C1017" s="109"/>
       <c r="D1017" s="110"/>
-      <c r="E1017" s="125"/>
+      <c r="E1017" s="121"/>
       <c r="F1017" s="110"/>
       <c r="G1017" s="112"/>
       <c r="H1017" s="112"/>
@@ -25796,7 +26032,7 @@
       <c r="N1017" s="113"/>
       <c r="O1017" s="116"/>
       <c r="P1017" s="119"/>
-      <c r="Q1017" s="126"/>
+      <c r="Q1017" s="122"/>
       <c r="R1017" s="119"/>
     </row>
     <row r="1018" spans="1:18" ht="29.25" customHeight="1">
@@ -25804,7 +26040,7 @@
       <c r="B1018" s="108"/>
       <c r="C1018" s="109"/>
       <c r="D1018" s="110"/>
-      <c r="E1018" s="125"/>
+      <c r="E1018" s="111"/>
       <c r="F1018" s="110"/>
       <c r="G1018" s="112"/>
       <c r="H1018" s="112"/>
@@ -25816,22 +26052,142 @@
       <c r="N1018" s="113"/>
       <c r="O1018" s="116"/>
       <c r="P1018" s="119"/>
-      <c r="Q1018" s="126"/>
+      <c r="Q1018" s="118"/>
       <c r="R1018" s="119"/>
     </row>
-    <row r="1019" spans="1:18" ht="29.25" customHeight="1"/>
+    <row r="1019" spans="1:18" ht="29.25" customHeight="1">
+      <c r="A1019" s="107"/>
+      <c r="B1019" s="108"/>
+      <c r="C1019" s="109"/>
+      <c r="D1019" s="110"/>
+      <c r="E1019" s="121"/>
+      <c r="F1019" s="110"/>
+      <c r="G1019" s="112"/>
+      <c r="H1019" s="112"/>
+      <c r="I1019" s="113"/>
+      <c r="J1019" s="114"/>
+      <c r="K1019" s="114"/>
+      <c r="L1019" s="114"/>
+      <c r="M1019" s="120"/>
+      <c r="N1019" s="113"/>
+      <c r="O1019" s="116"/>
+      <c r="P1019" s="119"/>
+      <c r="Q1019" s="122"/>
+      <c r="R1019" s="119"/>
+    </row>
+    <row r="1020" spans="1:18" ht="29.25" customHeight="1">
+      <c r="A1020" s="107"/>
+      <c r="B1020" s="108"/>
+      <c r="C1020" s="109"/>
+      <c r="D1020" s="110"/>
+      <c r="E1020" s="111"/>
+      <c r="F1020" s="110"/>
+      <c r="G1020" s="112"/>
+      <c r="H1020" s="112"/>
+      <c r="I1020" s="113"/>
+      <c r="J1020" s="114"/>
+      <c r="K1020" s="114"/>
+      <c r="L1020" s="114"/>
+      <c r="M1020" s="120"/>
+      <c r="N1020" s="113"/>
+      <c r="O1020" s="116"/>
+      <c r="P1020" s="119"/>
+      <c r="Q1020" s="118"/>
+      <c r="R1020" s="119"/>
+    </row>
+    <row r="1021" spans="1:18" ht="29.25" customHeight="1">
+      <c r="A1021" s="107"/>
+      <c r="B1021" s="108"/>
+      <c r="C1021" s="109"/>
+      <c r="D1021" s="110"/>
+      <c r="E1021" s="121"/>
+      <c r="F1021" s="110"/>
+      <c r="G1021" s="112"/>
+      <c r="H1021" s="112"/>
+      <c r="I1021" s="113"/>
+      <c r="J1021" s="114"/>
+      <c r="K1021" s="114"/>
+      <c r="L1021" s="114"/>
+      <c r="M1021" s="120"/>
+      <c r="N1021" s="113"/>
+      <c r="O1021" s="116"/>
+      <c r="P1021" s="119"/>
+      <c r="Q1021" s="122"/>
+      <c r="R1021" s="119"/>
+    </row>
+    <row r="1022" spans="1:18" ht="29.25" customHeight="1">
+      <c r="A1022" s="107"/>
+      <c r="B1022" s="108"/>
+      <c r="C1022" s="109"/>
+      <c r="D1022" s="110"/>
+      <c r="E1022" s="123"/>
+      <c r="F1022" s="110"/>
+      <c r="G1022" s="112"/>
+      <c r="H1022" s="112"/>
+      <c r="I1022" s="113"/>
+      <c r="J1022" s="114"/>
+      <c r="K1022" s="114"/>
+      <c r="L1022" s="114"/>
+      <c r="M1022" s="120"/>
+      <c r="N1022" s="113"/>
+      <c r="O1022" s="116"/>
+      <c r="P1022" s="119"/>
+      <c r="Q1022" s="124"/>
+      <c r="R1022" s="119"/>
+    </row>
+    <row r="1023" spans="1:18" ht="29.25" customHeight="1">
+      <c r="A1023" s="107"/>
+      <c r="B1023" s="108"/>
+      <c r="C1023" s="109"/>
+      <c r="D1023" s="110"/>
+      <c r="E1023" s="125"/>
+      <c r="F1023" s="110"/>
+      <c r="G1023" s="112"/>
+      <c r="H1023" s="112"/>
+      <c r="I1023" s="113"/>
+      <c r="J1023" s="114"/>
+      <c r="K1023" s="114"/>
+      <c r="L1023" s="114"/>
+      <c r="M1023" s="120"/>
+      <c r="N1023" s="113"/>
+      <c r="O1023" s="116"/>
+      <c r="P1023" s="119"/>
+      <c r="Q1023" s="126"/>
+      <c r="R1023" s="119"/>
+    </row>
+    <row r="1024" spans="1:18" ht="29.25" customHeight="1">
+      <c r="A1024" s="107"/>
+      <c r="B1024" s="108"/>
+      <c r="C1024" s="109"/>
+      <c r="D1024" s="110"/>
+      <c r="E1024" s="125"/>
+      <c r="F1024" s="110"/>
+      <c r="G1024" s="112"/>
+      <c r="H1024" s="112"/>
+      <c r="I1024" s="113"/>
+      <c r="J1024" s="114"/>
+      <c r="K1024" s="114"/>
+      <c r="L1024" s="114"/>
+      <c r="M1024" s="120"/>
+      <c r="N1024" s="113"/>
+      <c r="O1024" s="116"/>
+      <c r="P1024" s="119"/>
+      <c r="Q1024" s="126"/>
+      <c r="R1024" s="119"/>
+    </row>
+    <row r="1025" ht="29.25" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="B2:B1019">
+  <conditionalFormatting sqref="B2:B1025">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>COUNTIF($B$2:$B$1009,B2)&gt;1</formula>
+      <formula>COUNTIF($B$2:$B$1015,B2)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="Q2:Q1018"/>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L1018 N2:O1018">
+    <dataValidation allowBlank="1" showDropDown="1" sqref="Q2:Q1024"/>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L1024 N2:O1024">
       <formula1>OR(NOT(ISERROR(DATEVALUE(I2))), AND(ISNUMBER(I2), LEFT(CELL("format", I2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F1018">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F1024">
       <formula1>"FINALIZADO,EN PROCESO,PAUSADO,EN TEST,PENDIENTE,PRUEBAS CLIENTE,PENDIENTE CLIENTE,PRUEBAS IMAGINE,PASO A PRODUCCION"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 05 Diciembre
</commit_message>
<xml_diff>
--- a/Alfa.xlsx
+++ b/Alfa.xlsx
@@ -18,7 +18,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'EN PROCESO (Alfa)'!$A$1:$R$1028</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'EN PROCESO (Alfa)'!$A$1:$R$1032</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="408">
   <si>
     <t>Asignado a</t>
   </si>
@@ -1466,7 +1466,9 @@
   </si>
   <si>
     <t xml:space="preserve">26/11/2025: En la sesión tenia con el cliente surgieron algunos temas de mejoras, se procedió a realizar los ajustes requeridos y se solucionaron los issus reportados.  
-28/11/2025: se realiza sesión para revisar los temas propuestos en las sesiones pasadas, se realizan las pruebas satisfactoriamente, a excepción de dos cosas que no realizo cierre del mes de junio y se debe ajustar el campo rubro ya que hay formatos donde llega item-rubro. </t>
+28/11/2025: se realiza sesión para revisar los temas propuestos en las sesiones pasadas, se realizan las pruebas satisfactoriamente, a excepción de dos cosas que no realizo cierre del mes de junio y se debe ajustar el campo rubro ya que hay formatos donde llega item-rubro. 
+04/12/2025: Se tuvo reunión con el cliente para la realización de pruebas por parte de la funcionaria que realiza los pagos, y pidieron ajuste en los formatos de plus, sipren y tesoreria.
+Se realizo el respectivo a ajuste. </t>
   </si>
   <si>
     <t>Img_2025_029</t>
@@ -1493,7 +1495,56 @@
     <t>Validar cambios que se requieren para la elaboraciòn de Cronograma, generaciòn de OD</t>
   </si>
   <si>
-    <t>01/12/2025: Se requiere que el plan de trabajo se pueda agendar las ordene de servicio por periodo y ajustar tarifa para que tenga parametrización mas como lo es temática.  El dia de hoy se analizara el requerimiento con el jefe de unidad.</t>
+    <t>01/12/2025: Se requiere que el plan de trabajo se pueda agendar las ordene de servicio por periodo y ajustar tarifa para que tenga parametrización mas como lo es temática.  El dia de hoy se analizara el requerimiento con el jefe de unidad.
+02/12/2025: Se estuvo analizando este nuevo ajuste el módulo de plan de trabajo, donde se requieren varios ajustes al módulo en cuanto a parámetros, productos, cronogramas y validar si no afecta modulo de profesionales.   
+03/12/2025: Se realizó acompañamiento al jefe de unidad en la construcción del mockup del modulo de productos  y afinando estos nuevos ajustes.
+Posterior se tuvo reunión con el cliente, para mostrar los mockups de cómo va ir quedando los modulo y despejar dudas frente a estos nuevos cambios.</t>
+  </si>
+  <si>
+    <t>Img_2025_030</t>
+  </si>
+  <si>
+    <t>Correspondencia - Soporte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/12/2025: Se presenta issu en el cargue de archivos debido a que el sistema tiene limitado el cargue 2MB, por lo tanto, de aumenta tamaño a 5MB </t>
+  </si>
+  <si>
+    <t>PRV_2025_036</t>
+  </si>
+  <si>
+    <t>Soporte Previsionales</t>
+  </si>
+  <si>
+    <t>Asignar permisos</t>
+  </si>
+  <si>
+    <t>03/12/2025: Solicitan asignar nuevos permisos a dos integrantes a los modulos que actualmente maneja Blanca.</t>
+  </si>
+  <si>
+    <t>SST_2025_018</t>
+  </si>
+  <si>
+    <t>Plan de Trabajo ALFASST - Parámetros</t>
+  </si>
+  <si>
+    <t>Validar parámetros</t>
+  </si>
+  <si>
+    <t>05/12/2025: Se estuvo ajustando el módulo de productos, para que en los parametros de temáticas se puede asociar a un programa.
+Para las actividades se les puede asociar un valor.</t>
+  </si>
+  <si>
+    <t>PRV_2025_037</t>
+  </si>
+  <si>
+    <t>Soporte Previsionales - Cambio de Contraseña</t>
+  </si>
+  <si>
+    <t>Validar cambios de contraseña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/12/2025: Nos notifican que esta teniendo problemas con el cambio de contraseña, se realiza refactorización de url y se le notifica al cliente. </t>
   </si>
 </sst>
 </file>
@@ -2399,8 +2450,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla" displayName="Tabla" ref="A1:R1028">
-  <autoFilter ref="A1:R1028"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla" displayName="Tabla" ref="A1:R1032">
+  <autoFilter ref="A1:R1032"/>
   <tableColumns count="18">
     <tableColumn id="1" name="Asignado a"/>
     <tableColumn id="2" name="# REQ"/>
@@ -2691,10 +2742,10 @@
   <sheetPr>
     <tabColor rgb="FFCC0000"/>
   </sheetPr>
-  <dimension ref="A1:R1029"/>
+  <dimension ref="A1:R1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -4792,7 +4843,7 @@
       <c r="L43" s="68"/>
       <c r="M43" s="69">
         <f ca="1">IF(ISBLANK(L43), NETWORKDAYS(J43, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J43, L43, [1]Hoja2!$A$1:$A$18))</f>
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="N43" s="70"/>
       <c r="O43" s="71"/>
@@ -7543,7 +7594,7 @@
       <c r="L100" s="75"/>
       <c r="M100" s="90">
         <f ca="1">IF(ISBLANK(L100), NETWORKDAYS(J100, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J100, L100, [1]Hoja2!$A$1:$A$18))</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="N100" s="91"/>
       <c r="O100" s="92"/>
@@ -7786,7 +7837,7 @@
       <c r="L105" s="75"/>
       <c r="M105" s="90">
         <f ca="1">IF(ISBLANK(L105), NETWORKDAYS(J105, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J105, L105, [1]Hoja2!$A$1:$A$18))</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="N105" s="91"/>
       <c r="O105" s="92"/>
@@ -7962,10 +8013,10 @@
         <v>21</v>
       </c>
       <c r="F109" s="65" t="s">
-        <v>161</v>
+        <v>22</v>
       </c>
       <c r="G109" s="82">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H109" s="78"/>
       <c r="I109" s="102">
@@ -7978,11 +8029,11 @@
         <v>45988</v>
       </c>
       <c r="L109" s="103">
-        <v>45988</v>
+        <v>45995</v>
       </c>
       <c r="M109" s="98">
         <f ca="1">IF(ISBLANK(L109), NETWORKDAYS(J109, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J109, L109, [1]Hoja2!$A$1:$A$18))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N109" s="70"/>
       <c r="O109" s="71"/>
@@ -8027,7 +8078,7 @@
       <c r="L110" s="103"/>
       <c r="M110" s="98">
         <f ca="1">IF(ISBLANK(L110), NETWORKDAYS(J110, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J110, L110, [1]Hoja2!$A$1:$A$18))</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N110" s="70"/>
       <c r="O110" s="71"/>
@@ -8059,7 +8110,7 @@
         <v>161</v>
       </c>
       <c r="G111" s="88">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H111" s="89"/>
       <c r="I111" s="94">
@@ -8072,7 +8123,7 @@
       <c r="L111" s="75"/>
       <c r="M111" s="90">
         <f ca="1">IF(ISBLANK(L111), NETWORKDAYS(J111, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J111, L111, [1]Hoja2!$A$1:$A$18))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N111" s="91"/>
       <c r="O111" s="92"/>
@@ -8085,84 +8136,200 @@
       <c r="R111" s="72"/>
     </row>
     <row r="112" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A112" s="107"/>
-      <c r="B112" s="108"/>
-      <c r="C112" s="109"/>
-      <c r="D112" s="110"/>
-      <c r="E112" s="111"/>
-      <c r="F112" s="110"/>
-      <c r="G112" s="112"/>
-      <c r="H112" s="112"/>
-      <c r="I112" s="113"/>
-      <c r="J112" s="114"/>
-      <c r="K112" s="114"/>
-      <c r="L112" s="114"/>
-      <c r="M112" s="115"/>
-      <c r="N112" s="113"/>
-      <c r="O112" s="116"/>
-      <c r="P112" s="117"/>
-      <c r="Q112" s="118"/>
-      <c r="R112" s="119"/>
+      <c r="A112" s="95" t="s">
+        <v>18</v>
+      </c>
+      <c r="B112" s="81" t="s">
+        <v>393</v>
+      </c>
+      <c r="C112" s="96" t="s">
+        <v>394</v>
+      </c>
+      <c r="D112" s="63" t="s">
+        <v>386</v>
+      </c>
+      <c r="E112" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="F112" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="G112" s="82">
+        <v>100</v>
+      </c>
+      <c r="H112" s="78"/>
+      <c r="I112" s="102">
+        <v>45994</v>
+      </c>
+      <c r="J112" s="103">
+        <v>45994</v>
+      </c>
+      <c r="K112" s="103">
+        <v>45994</v>
+      </c>
+      <c r="L112" s="103">
+        <v>45994</v>
+      </c>
+      <c r="M112" s="98">
+        <f ca="1">IF(ISBLANK(L112), NETWORKDAYS(J112, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J112, L112, [1]Hoja2!$A$1:$A$18))</f>
+        <v>1</v>
+      </c>
+      <c r="N112" s="70"/>
+      <c r="O112" s="71"/>
+      <c r="P112" s="104" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q112" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="R112" s="80"/>
     </row>
     <row r="113" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A113" s="107"/>
-      <c r="B113" s="108"/>
-      <c r="C113" s="109"/>
-      <c r="D113" s="110"/>
-      <c r="E113" s="111"/>
-      <c r="F113" s="110"/>
-      <c r="G113" s="112"/>
-      <c r="H113" s="112"/>
-      <c r="I113" s="113"/>
-      <c r="J113" s="114"/>
-      <c r="K113" s="114"/>
-      <c r="L113" s="114"/>
-      <c r="M113" s="120"/>
-      <c r="N113" s="113"/>
-      <c r="O113" s="116"/>
-      <c r="P113" s="119"/>
-      <c r="Q113" s="118"/>
-      <c r="R113" s="119"/>
+      <c r="A113" s="95" t="s">
+        <v>18</v>
+      </c>
+      <c r="B113" s="64" t="s">
+        <v>396</v>
+      </c>
+      <c r="C113" s="62" t="s">
+        <v>397</v>
+      </c>
+      <c r="D113" s="74" t="s">
+        <v>398</v>
+      </c>
+      <c r="E113" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="F113" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="G113" s="82">
+        <v>100</v>
+      </c>
+      <c r="H113" s="78"/>
+      <c r="I113" s="102">
+        <v>45994</v>
+      </c>
+      <c r="J113" s="103">
+        <v>45994</v>
+      </c>
+      <c r="K113" s="103">
+        <v>45994</v>
+      </c>
+      <c r="L113" s="103">
+        <v>45994</v>
+      </c>
+      <c r="M113" s="98">
+        <f ca="1">IF(ISBLANK(L113), NETWORKDAYS(J113, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J113, L113, [1]Hoja2!$A$1:$A$18))</f>
+        <v>1</v>
+      </c>
+      <c r="N113" s="70"/>
+      <c r="O113" s="71"/>
+      <c r="P113" s="104" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q113" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="R113" s="80"/>
     </row>
     <row r="114" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A114" s="107"/>
-      <c r="B114" s="108"/>
-      <c r="C114" s="109"/>
-      <c r="D114" s="110"/>
-      <c r="E114" s="111"/>
-      <c r="F114" s="110"/>
-      <c r="G114" s="112"/>
-      <c r="H114" s="112"/>
-      <c r="I114" s="113"/>
-      <c r="J114" s="114"/>
-      <c r="K114" s="114"/>
-      <c r="L114" s="114"/>
-      <c r="M114" s="120"/>
-      <c r="N114" s="113"/>
-      <c r="O114" s="116"/>
-      <c r="P114" s="119"/>
-      <c r="Q114" s="118"/>
-      <c r="R114" s="119"/>
+      <c r="A114" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="B114" s="64" t="s">
+        <v>400</v>
+      </c>
+      <c r="C114" s="86" t="s">
+        <v>401</v>
+      </c>
+      <c r="D114" s="100" t="s">
+        <v>402</v>
+      </c>
+      <c r="E114" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="F114" s="99" t="s">
+        <v>22</v>
+      </c>
+      <c r="G114" s="88">
+        <v>100</v>
+      </c>
+      <c r="H114" s="89"/>
+      <c r="I114" s="94">
+        <v>45995</v>
+      </c>
+      <c r="J114" s="75">
+        <v>45995</v>
+      </c>
+      <c r="K114" s="75">
+        <v>45996</v>
+      </c>
+      <c r="L114" s="75">
+        <v>45996</v>
+      </c>
+      <c r="M114" s="90">
+        <f ca="1">IF(ISBLANK(L114), NETWORKDAYS(J114, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J114, L114, [1]Hoja2!$A$1:$A$18))</f>
+        <v>2</v>
+      </c>
+      <c r="N114" s="91"/>
+      <c r="O114" s="92"/>
+      <c r="P114" s="76" t="s">
+        <v>403</v>
+      </c>
+      <c r="Q114" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="R114" s="72"/>
     </row>
     <row r="115" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A115" s="107"/>
-      <c r="B115" s="108"/>
-      <c r="C115" s="109"/>
-      <c r="D115" s="110"/>
-      <c r="E115" s="111"/>
-      <c r="F115" s="110"/>
-      <c r="G115" s="112"/>
-      <c r="H115" s="112"/>
-      <c r="I115" s="113"/>
-      <c r="J115" s="114"/>
-      <c r="K115" s="114"/>
-      <c r="L115" s="114"/>
-      <c r="M115" s="120"/>
-      <c r="N115" s="113"/>
-      <c r="O115" s="116"/>
-      <c r="P115" s="119"/>
-      <c r="Q115" s="118"/>
-      <c r="R115" s="119"/>
+      <c r="A115" s="95" t="s">
+        <v>18</v>
+      </c>
+      <c r="B115" s="64" t="s">
+        <v>404</v>
+      </c>
+      <c r="C115" s="62" t="s">
+        <v>405</v>
+      </c>
+      <c r="D115" s="74" t="s">
+        <v>406</v>
+      </c>
+      <c r="E115" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="F115" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="G115" s="82">
+        <v>100</v>
+      </c>
+      <c r="H115" s="78"/>
+      <c r="I115" s="102">
+        <v>45996</v>
+      </c>
+      <c r="J115" s="103">
+        <v>45996</v>
+      </c>
+      <c r="K115" s="103">
+        <v>45996</v>
+      </c>
+      <c r="L115" s="103">
+        <v>45996</v>
+      </c>
+      <c r="M115" s="98">
+        <f ca="1">IF(ISBLANK(L115), NETWORKDAYS(J115, TODAY(),[1]Hoja2!$A$1:$A$18), NETWORKDAYS(J115, L115, [1]Hoja2!$A$1:$A$18))</f>
+        <v>1</v>
+      </c>
+      <c r="N115" s="70"/>
+      <c r="O115" s="71"/>
+      <c r="P115" s="104" t="s">
+        <v>407</v>
+      </c>
+      <c r="Q115" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="R115" s="80"/>
     </row>
     <row r="116" spans="1:18" ht="29.25" customHeight="1">
       <c r="A116" s="107"/>
@@ -8177,10 +8344,10 @@
       <c r="J116" s="114"/>
       <c r="K116" s="114"/>
       <c r="L116" s="114"/>
-      <c r="M116" s="120"/>
+      <c r="M116" s="115"/>
       <c r="N116" s="113"/>
       <c r="O116" s="116"/>
-      <c r="P116" s="119"/>
+      <c r="P116" s="117"/>
       <c r="Q116" s="118"/>
       <c r="R116" s="119"/>
     </row>
@@ -8349,7 +8516,7 @@
       <c r="B125" s="108"/>
       <c r="C125" s="109"/>
       <c r="D125" s="110"/>
-      <c r="E125" s="121"/>
+      <c r="E125" s="111"/>
       <c r="F125" s="110"/>
       <c r="G125" s="112"/>
       <c r="H125" s="112"/>
@@ -8361,7 +8528,7 @@
       <c r="N125" s="113"/>
       <c r="O125" s="116"/>
       <c r="P125" s="119"/>
-      <c r="Q125" s="122"/>
+      <c r="Q125" s="118"/>
       <c r="R125" s="119"/>
     </row>
     <row r="126" spans="1:18" ht="29.25" customHeight="1">
@@ -8389,7 +8556,7 @@
       <c r="B127" s="108"/>
       <c r="C127" s="109"/>
       <c r="D127" s="110"/>
-      <c r="E127" s="121"/>
+      <c r="E127" s="111"/>
       <c r="F127" s="110"/>
       <c r="G127" s="112"/>
       <c r="H127" s="112"/>
@@ -8401,7 +8568,7 @@
       <c r="N127" s="113"/>
       <c r="O127" s="116"/>
       <c r="P127" s="119"/>
-      <c r="Q127" s="122"/>
+      <c r="Q127" s="118"/>
       <c r="R127" s="119"/>
     </row>
     <row r="128" spans="1:18" ht="29.25" customHeight="1">
@@ -26369,7 +26536,7 @@
       <c r="B1026" s="108"/>
       <c r="C1026" s="109"/>
       <c r="D1026" s="110"/>
-      <c r="E1026" s="123"/>
+      <c r="E1026" s="111"/>
       <c r="F1026" s="110"/>
       <c r="G1026" s="112"/>
       <c r="H1026" s="112"/>
@@ -26381,7 +26548,7 @@
       <c r="N1026" s="113"/>
       <c r="O1026" s="116"/>
       <c r="P1026" s="119"/>
-      <c r="Q1026" s="124"/>
+      <c r="Q1026" s="118"/>
       <c r="R1026" s="119"/>
     </row>
     <row r="1027" spans="1:18" ht="29.25" customHeight="1">
@@ -26389,7 +26556,7 @@
       <c r="B1027" s="108"/>
       <c r="C1027" s="109"/>
       <c r="D1027" s="110"/>
-      <c r="E1027" s="125"/>
+      <c r="E1027" s="121"/>
       <c r="F1027" s="110"/>
       <c r="G1027" s="112"/>
       <c r="H1027" s="112"/>
@@ -26401,7 +26568,7 @@
       <c r="N1027" s="113"/>
       <c r="O1027" s="116"/>
       <c r="P1027" s="119"/>
-      <c r="Q1027" s="126"/>
+      <c r="Q1027" s="122"/>
       <c r="R1027" s="119"/>
     </row>
     <row r="1028" spans="1:18" ht="29.25" customHeight="1">
@@ -26409,7 +26576,7 @@
       <c r="B1028" s="108"/>
       <c r="C1028" s="109"/>
       <c r="D1028" s="110"/>
-      <c r="E1028" s="125"/>
+      <c r="E1028" s="111"/>
       <c r="F1028" s="110"/>
       <c r="G1028" s="112"/>
       <c r="H1028" s="112"/>
@@ -26421,22 +26588,102 @@
       <c r="N1028" s="113"/>
       <c r="O1028" s="116"/>
       <c r="P1028" s="119"/>
-      <c r="Q1028" s="126"/>
+      <c r="Q1028" s="118"/>
       <c r="R1028" s="119"/>
     </row>
-    <row r="1029" spans="1:18" ht="29.25" customHeight="1"/>
+    <row r="1029" spans="1:18" ht="29.25" customHeight="1">
+      <c r="A1029" s="107"/>
+      <c r="B1029" s="108"/>
+      <c r="C1029" s="109"/>
+      <c r="D1029" s="110"/>
+      <c r="E1029" s="121"/>
+      <c r="F1029" s="110"/>
+      <c r="G1029" s="112"/>
+      <c r="H1029" s="112"/>
+      <c r="I1029" s="113"/>
+      <c r="J1029" s="114"/>
+      <c r="K1029" s="114"/>
+      <c r="L1029" s="114"/>
+      <c r="M1029" s="120"/>
+      <c r="N1029" s="113"/>
+      <c r="O1029" s="116"/>
+      <c r="P1029" s="119"/>
+      <c r="Q1029" s="122"/>
+      <c r="R1029" s="119"/>
+    </row>
+    <row r="1030" spans="1:18" ht="29.25" customHeight="1">
+      <c r="A1030" s="107"/>
+      <c r="B1030" s="108"/>
+      <c r="C1030" s="109"/>
+      <c r="D1030" s="110"/>
+      <c r="E1030" s="123"/>
+      <c r="F1030" s="110"/>
+      <c r="G1030" s="112"/>
+      <c r="H1030" s="112"/>
+      <c r="I1030" s="113"/>
+      <c r="J1030" s="114"/>
+      <c r="K1030" s="114"/>
+      <c r="L1030" s="114"/>
+      <c r="M1030" s="120"/>
+      <c r="N1030" s="113"/>
+      <c r="O1030" s="116"/>
+      <c r="P1030" s="119"/>
+      <c r="Q1030" s="124"/>
+      <c r="R1030" s="119"/>
+    </row>
+    <row r="1031" spans="1:18" ht="29.25" customHeight="1">
+      <c r="A1031" s="107"/>
+      <c r="B1031" s="108"/>
+      <c r="C1031" s="109"/>
+      <c r="D1031" s="110"/>
+      <c r="E1031" s="125"/>
+      <c r="F1031" s="110"/>
+      <c r="G1031" s="112"/>
+      <c r="H1031" s="112"/>
+      <c r="I1031" s="113"/>
+      <c r="J1031" s="114"/>
+      <c r="K1031" s="114"/>
+      <c r="L1031" s="114"/>
+      <c r="M1031" s="120"/>
+      <c r="N1031" s="113"/>
+      <c r="O1031" s="116"/>
+      <c r="P1031" s="119"/>
+      <c r="Q1031" s="126"/>
+      <c r="R1031" s="119"/>
+    </row>
+    <row r="1032" spans="1:18" ht="29.25" customHeight="1">
+      <c r="A1032" s="107"/>
+      <c r="B1032" s="108"/>
+      <c r="C1032" s="109"/>
+      <c r="D1032" s="110"/>
+      <c r="E1032" s="125"/>
+      <c r="F1032" s="110"/>
+      <c r="G1032" s="112"/>
+      <c r="H1032" s="112"/>
+      <c r="I1032" s="113"/>
+      <c r="J1032" s="114"/>
+      <c r="K1032" s="114"/>
+      <c r="L1032" s="114"/>
+      <c r="M1032" s="120"/>
+      <c r="N1032" s="113"/>
+      <c r="O1032" s="116"/>
+      <c r="P1032" s="119"/>
+      <c r="Q1032" s="126"/>
+      <c r="R1032" s="119"/>
+    </row>
+    <row r="1033" spans="1:18" ht="29.25" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="B2:B1029">
+  <conditionalFormatting sqref="B2:B1033">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>COUNTIF($B$2:$B$1019,B2)&gt;1</formula>
+      <formula>COUNTIF($B$2:$B$1023,B2)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="Q2:Q1028"/>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L1028 N2:O1028">
+    <dataValidation allowBlank="1" showDropDown="1" sqref="Q2:Q1032"/>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L1032 N2:O1032">
       <formula1>OR(NOT(ISERROR(DATEVALUE(I2))), AND(ISNUMBER(I2), LEFT(CELL("format", I2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F1028">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F1032">
       <formula1>"FINALIZADO,EN PROCESO,PAUSADO,EN TEST,PENDIENTE,PRUEBAS CLIENTE,PENDIENTE CLIENTE,PRUEBAS IMAGINE,PASO A PRODUCCION"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 13 de febrero 2026
</commit_message>
<xml_diff>
--- a/Alfa.xlsx
+++ b/Alfa.xlsx
@@ -17,9 +17,6 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'EN PROCESO (Alfa)'!$A$1:$S$124</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2600,7 +2597,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla" displayName="Tabla" ref="A1:S124">
-  <autoFilter ref="A1:S124"/>
   <tableColumns count="19">
     <tableColumn id="1" name="Asignado a"/>
     <tableColumn id="2" name="# REQ"/>
@@ -2896,7 +2892,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -8903,7 +8899,7 @@
       NETWORKDAYS(J105,L105,[1]fESTIVOS!$A$2:$A$53)
    )
 )</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="N105" s="83"/>
       <c r="O105" s="83"/>
@@ -9537,7 +9533,7 @@
       NETWORKDAYS(J116,L116,[1]fESTIVOS!$A$2:$A$53)
    )
 )</f>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="N116" s="83"/>
       <c r="O116" s="83"/>
@@ -9881,7 +9877,7 @@
       NETWORKDAYS(J122,L122,[1]fESTIVOS!$A$2:$A$53)
    )
 )</f>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="N122" s="67"/>
       <c r="O122" s="67"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 24 de febrero 2026
</commit_message>
<xml_diff>
--- a/Alfa.xlsx
+++ b/Alfa.xlsx
@@ -3065,8 +3065,8 @@
   <dimension ref="A1:S1054"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A134" sqref="A134"/>
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>